<commit_message>
ESPixel now 12V or 5V
Added 5V reg for 12V pixel operation.
</commit_message>
<xml_diff>
--- a/ESPixelGECEBOM.xlsx
+++ b/ESPixelGECEBOM.xlsx
@@ -12,6 +12,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -486,7 +487,7 @@
   <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -544,14 +545,14 @@
         <v>0.62</v>
       </c>
       <c r="F2">
-        <f>E2*D2</f>
+        <f t="shared" ref="F2:F9" si="0">E2*D2</f>
         <v>0.62</v>
       </c>
       <c r="G2">
         <v>0.27</v>
       </c>
       <c r="H2">
-        <f>G2*100*D2</f>
+        <f t="shared" ref="H2:H9" si="1">G2*100*D2</f>
         <v>27</v>
       </c>
       <c r="I2" s="1"/>
@@ -573,14 +574,14 @@
         <v>0.23</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F5" si="0">E3*D3</f>
+        <f t="shared" si="0"/>
         <v>0.23</v>
       </c>
       <c r="G3">
         <v>8.6999999999999994E-2</v>
       </c>
       <c r="H3">
-        <f t="shared" ref="H3:H5" si="1">G3*100*D3</f>
+        <f t="shared" si="1"/>
         <v>8.6999999999999993</v>
       </c>
       <c r="I3" s="1"/>
@@ -659,14 +660,14 @@
         <v>0.1</v>
       </c>
       <c r="F6">
-        <f>E6*D6</f>
+        <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
       <c r="G6">
         <v>0.02</v>
       </c>
       <c r="H6">
-        <f>G6*100*D6</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
     </row>
@@ -687,14 +688,14 @@
         <v>2.34</v>
       </c>
       <c r="F7">
-        <f>E7*D7</f>
+        <f t="shared" si="0"/>
         <v>0.7722</v>
       </c>
       <c r="G7">
         <v>1.72</v>
       </c>
       <c r="H7">
-        <f>G7*100*D7</f>
+        <f t="shared" si="1"/>
         <v>56.760000000000005</v>
       </c>
     </row>
@@ -715,14 +716,14 @@
         <v>0.1</v>
       </c>
       <c r="F8">
-        <f>E8*D8</f>
+        <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
       <c r="G8">
         <v>2.24E-2</v>
       </c>
       <c r="H8">
-        <f>G8*100*D8</f>
+        <f t="shared" si="1"/>
         <v>2.2399999999999998</v>
       </c>
     </row>
@@ -743,14 +744,14 @@
         <v>0.11</v>
       </c>
       <c r="F9">
-        <f>E9*D9</f>
+        <f t="shared" si="0"/>
         <v>0.11</v>
       </c>
       <c r="G9">
         <v>0.08</v>
       </c>
       <c r="H9">
-        <f>G9*100*D9</f>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
     </row>

</xml_diff>